<commit_message>
added Enemy AI (Mattis stinkt)
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Desktop\Project Pink Spyda\infoProjekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oem\Desktop\infoProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6DB294-E047-423C-9EE3-028A8D0B09C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CDEDE1-334E-408D-9781-42B8E3DFE9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D947EC2-8678-403C-BE8C-FA3415FBAF11}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D947EC2-8678-403C-BE8C-FA3415FBAF11}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Types:</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>ceiling</t>
+  </si>
+  <si>
+    <t>RifleBullet</t>
+  </si>
+  <si>
+    <t>Melee "Bullet"</t>
   </si>
 </sst>
 </file>
@@ -442,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E48337-378F-4F66-BC89-4755B4EE393E}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,6 +529,22 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>